<commit_message>
Condicional Cambio de plan
</commit_message>
<xml_diff>
--- a/registers.xlsx
+++ b/registers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ipupo\Documents\GitHub\Automatizaci-nTFNU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{176E6025-CB46-44CB-B534-DABBB6CDC994}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC569B94-5613-417E-A8BA-3AC20D79785B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14790" windowHeight="7650" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14790" windowHeight="7650" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="POTENTIAL-RESCLIENTS" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="37">
   <si>
     <t>UAT</t>
   </si>
@@ -133,16 +133,13 @@
     <t>PLC239</t>
   </si>
   <si>
-    <t>PLR282</t>
-  </si>
-  <si>
     <t>PLTTEF</t>
   </si>
   <si>
-    <t>89598071102044548316</t>
-  </si>
-  <si>
-    <t>95879202</t>
+    <t>95879365</t>
+  </si>
+  <si>
+    <t>89598071102044553175</t>
   </si>
 </sst>
 </file>
@@ -1094,7 +1091,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1321,13 +1318,13 @@
         <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>36</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1386,8 +1383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ADDCCCF-6AB2-46AA-A7AA-8F4CA3727986}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1422,10 +1419,10 @@
         <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1479,7 +1476,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FCFAA35-B389-4AC3-B2A7-BC50E5D70A93}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>

</xml_diff>